<commit_message>
other params and lil improvements
</commit_message>
<xml_diff>
--- a/tables/tableOtherParameter.xlsx
+++ b/tables/tableOtherParameter.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Godovova\MATLAB_Godovova\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\greatuniter\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67146CB6-534A-4A2E-AC43-CCC16FDDA138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="-17850" yWindow="2025" windowWidth="16200" windowHeight="9360" tabRatio="861" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
     <sheet name="Criteria" sheetId="3" r:id="rId2"/>
     <sheet name="Sample" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>ФИО проверяющего</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Фамилия И.О.</t>
-  </si>
-  <si>
-    <t>Ethernet</t>
-  </si>
-  <si>
-    <t>работает/не работает</t>
   </si>
   <si>
     <t>Температура внешней среды, °С</t>
@@ -63,9 +57,6 @@
   </si>
   <si>
     <t>Ток холостого хода, А</t>
-  </si>
-  <si>
-    <t>Максимальный потребляемый ток, А</t>
   </si>
   <si>
     <t>Therm_LD4</t>
@@ -155,19 +146,19 @@
     <t>3.3V_DAC_ADC</t>
   </si>
   <si>
-    <t>value, V</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +250,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -285,9 +276,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,9 +289,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="3"/>
-    <cellStyle name="Стиль 1" xfId="1"/>
-    <cellStyle name="Стиль 2" xfId="2"/>
+    <cellStyle name="Обычный 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Стиль 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Стиль 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -357,7 +345,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Стиль таблицы 1" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Стиль таблицы 1" pivot="0" count="2">
+    <tableStyle name="Стиль таблицы 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
@@ -635,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -649,487 +637,485 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19" style="10" customWidth="1"/>
-    <col min="3" max="5" width="9" style="10" customWidth="1"/>
-    <col min="6" max="11" width="11.7109375" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="10"/>
+    <col min="1" max="1" width="19.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19" style="9" customWidth="1"/>
+    <col min="3" max="5" width="9" style="9" customWidth="1"/>
+    <col min="6" max="11" width="11.7109375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>41</v>
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="10">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9">
         <f>E2*0.9</f>
         <v>2.2410000000000001</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <f>E2*1.1</f>
         <v>2.7390000000000003</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9">
         <v>0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>0.1</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="10">
-        <f t="shared" ref="C3:C25" si="0">E4*0.9</f>
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ref="C4:C25" si="0">E4*0.9</f>
         <v>2.2410000000000001</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" ref="D3:D25" si="1">E4*1.1</f>
+      <c r="D4" s="9">
+        <f t="shared" ref="D4:D25" si="1">E4*1.1</f>
         <v>2.7390000000000003</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="A5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.1</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="A8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.1</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="9">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9">
         <f t="shared" si="0"/>
         <v>1.512</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f t="shared" si="1"/>
         <v>1.8480000000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>1.68</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="A11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>1.512</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <f t="shared" si="1"/>
         <v>1.8480000000000001</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>1.68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>1.512</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f t="shared" si="1"/>
         <v>1.8480000000000001</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>1.68</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10">
+      <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
         <v>1.512</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <f t="shared" si="1"/>
         <v>1.8480000000000001</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>1.68</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="10">
-        <f t="shared" si="0"/>
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="D14" s="10">
-        <f t="shared" si="1"/>
-        <v>0.28600000000000003</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0.26</v>
+      <c r="A14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="10">
+      <c r="A15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="9">
         <f t="shared" si="0"/>
         <v>1.296</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f t="shared" si="1"/>
         <v>1.5840000000000001</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>1.44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="10">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="9">
         <f t="shared" si="0"/>
         <v>1.5209999999999999</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f t="shared" si="1"/>
         <v>1.859</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>1.69</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="10">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9">
         <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <f t="shared" si="1"/>
         <v>1.87</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>1.7</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="10">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="9">
         <f t="shared" si="0"/>
         <v>1.5029999999999999</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <f t="shared" si="1"/>
         <v>1.837</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>1.67</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="9">
         <f t="shared" si="0"/>
         <v>1.107</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <f t="shared" si="1"/>
         <v>1.353</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>1.23</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9">
         <f t="shared" si="0"/>
         <v>1.5029999999999999</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <f t="shared" si="1"/>
         <v>1.837</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>1.67</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="10">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9">
         <f t="shared" si="0"/>
         <v>1.107</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <f t="shared" si="1"/>
         <v>1.353</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>1.23</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="9">
         <f t="shared" si="0"/>
         <v>1.5029999999999999</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <f t="shared" si="1"/>
         <v>1.837</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>1.67</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="10">
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="9">
         <f t="shared" si="0"/>
         <v>1.107</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <f t="shared" si="1"/>
         <v>1.353</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>1.23</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="10">
+      <c r="A24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="9">
         <f t="shared" si="0"/>
         <v>1.107</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <f t="shared" si="1"/>
         <v>1.353</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>1.23</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="10">
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="9">
         <f t="shared" si="0"/>
         <v>1.5029999999999999</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <f t="shared" si="1"/>
         <v>1.837</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>1.67</v>
       </c>
     </row>
@@ -1139,11 +1125,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BT48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BT46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1">
         <v>11</v>
@@ -1249,9 +1235,7 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="4"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1323,7 +1307,7 @@
     </row>
     <row r="5" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
@@ -1397,7 +1381,7 @@
     </row>
     <row r="6" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="4"/>
@@ -1471,7 +1455,7 @@
     </row>
     <row r="7" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
@@ -1545,9 +1529,9 @@
     </row>
     <row r="8" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1617,12 +1601,14 @@
       <c r="BQ8" s="3"/>
       <c r="BR8" s="3"/>
     </row>
-    <row r="9" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="4"/>
+    <row r="9" spans="1:72" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1690,13 +1676,15 @@
       <c r="BP9" s="3"/>
       <c r="BQ9" s="3"/>
       <c r="BR9" s="3"/>
+      <c r="BS9" s="2"/>
+      <c r="BT9" s="2"/>
     </row>
     <row r="10" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1764,14 +1752,14 @@
       <c r="BP10" s="3"/>
       <c r="BQ10" s="3"/>
       <c r="BR10" s="3"/>
-    </row>
-    <row r="11" spans="1:72" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="BS10" s="2"/>
+      <c r="BT10" s="2"/>
+    </row>
+    <row r="11" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1844,8 +1832,8 @@
       <c r="BT11" s="2"/>
     </row>
     <row r="12" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>14</v>
+      <c r="A12" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1916,12 +1904,10 @@
       <c r="BP12" s="3"/>
       <c r="BQ12" s="3"/>
       <c r="BR12" s="3"/>
-      <c r="BS12" s="2"/>
-      <c r="BT12" s="2"/>
     </row>
     <row r="13" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>19</v>
+      <c r="A13" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1992,12 +1978,10 @@
       <c r="BP13" s="3"/>
       <c r="BQ13" s="3"/>
       <c r="BR13" s="3"/>
-      <c r="BS13" s="2"/>
-      <c r="BT13" s="2"/>
     </row>
     <row r="14" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>12</v>
+      <c r="A14" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2070,8 +2054,8 @@
       <c r="BR14" s="3"/>
     </row>
     <row r="15" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>18</v>
+      <c r="A15" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2144,7 +2128,7 @@
       <c r="BR15" s="3"/>
     </row>
     <row r="16" spans="1:72" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3"/>
@@ -2218,8 +2202,8 @@
       <c r="BR16" s="3"/>
     </row>
     <row r="17" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
+      <c r="A17" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2292,8 +2276,8 @@
       <c r="BR17" s="3"/>
     </row>
     <row r="18" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>20</v>
+      <c r="A18" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2366,8 +2350,8 @@
       <c r="BR18" s="3"/>
     </row>
     <row r="19" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>13</v>
+      <c r="A19" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2440,8 +2424,8 @@
       <c r="BR19" s="3"/>
     </row>
     <row r="20" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>27</v>
+      <c r="A20" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2514,8 +2498,8 @@
       <c r="BR20" s="3"/>
     </row>
     <row r="21" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>28</v>
+      <c r="A21" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2588,8 +2572,8 @@
       <c r="BR21" s="3"/>
     </row>
     <row r="22" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>29</v>
+      <c r="A22" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2662,8 +2646,8 @@
       <c r="BR22" s="3"/>
     </row>
     <row r="23" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>30</v>
+      <c r="A23" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2736,8 +2720,8 @@
       <c r="BR23" s="3"/>
     </row>
     <row r="24" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>26</v>
+      <c r="A24" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2810,8 +2794,8 @@
       <c r="BR24" s="3"/>
     </row>
     <row r="25" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>15</v>
+      <c r="A25" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2884,8 +2868,8 @@
       <c r="BR25" s="3"/>
     </row>
     <row r="26" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>31</v>
+      <c r="A26" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2958,8 +2942,8 @@
       <c r="BR26" s="3"/>
     </row>
     <row r="27" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>32</v>
+      <c r="A27" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3032,8 +3016,8 @@
       <c r="BR27" s="3"/>
     </row>
     <row r="28" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>33</v>
+      <c r="A28" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3106,8 +3090,8 @@
       <c r="BR28" s="3"/>
     </row>
     <row r="29" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>34</v>
+      <c r="A29" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3180,8 +3164,8 @@
       <c r="BR29" s="3"/>
     </row>
     <row r="30" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>35</v>
+      <c r="A30" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3254,8 +3238,8 @@
       <c r="BR30" s="3"/>
     </row>
     <row r="31" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>36</v>
+      <c r="A31" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -3328,8 +3312,8 @@
       <c r="BR31" s="3"/>
     </row>
     <row r="32" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>37</v>
+      <c r="A32" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -3402,8 +3386,8 @@
       <c r="BR32" s="3"/>
     </row>
     <row r="33" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>38</v>
+      <c r="A33" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3475,10 +3459,7 @@
       <c r="BQ33" s="3"/>
       <c r="BR33" s="3"/>
     </row>
-    <row r="34" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>39</v>
-      </c>
+    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -3549,10 +3530,7 @@
       <c r="BQ34" s="3"/>
       <c r="BR34" s="3"/>
     </row>
-    <row r="35" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>40</v>
-      </c>
+    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4404,148 +4382,6 @@
       <c r="BQ46" s="3"/>
       <c r="BR46" s="3"/>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="3"/>
-      <c r="AC47" s="3"/>
-      <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="3"/>
-      <c r="AG47" s="3"/>
-      <c r="AH47" s="3"/>
-      <c r="AI47" s="3"/>
-      <c r="AJ47" s="3"/>
-      <c r="AK47" s="3"/>
-      <c r="AL47" s="3"/>
-      <c r="AM47" s="3"/>
-      <c r="AN47" s="3"/>
-      <c r="AO47" s="3"/>
-      <c r="AP47" s="3"/>
-      <c r="AQ47" s="3"/>
-      <c r="AR47" s="3"/>
-      <c r="AS47" s="3"/>
-      <c r="AT47" s="3"/>
-      <c r="AU47" s="3"/>
-      <c r="AV47" s="3"/>
-      <c r="AW47" s="3"/>
-      <c r="AX47" s="3"/>
-      <c r="AY47" s="3"/>
-      <c r="AZ47" s="3"/>
-      <c r="BA47" s="3"/>
-      <c r="BB47" s="3"/>
-      <c r="BC47" s="3"/>
-      <c r="BD47" s="3"/>
-      <c r="BE47" s="3"/>
-      <c r="BF47" s="3"/>
-      <c r="BG47" s="3"/>
-      <c r="BH47" s="3"/>
-      <c r="BI47" s="3"/>
-      <c r="BJ47" s="3"/>
-      <c r="BK47" s="3"/>
-      <c r="BL47" s="3"/>
-      <c r="BM47" s="3"/>
-      <c r="BN47" s="3"/>
-      <c r="BO47" s="3"/>
-      <c r="BP47" s="3"/>
-      <c r="BQ47" s="3"/>
-      <c r="BR47" s="3"/>
-    </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="3"/>
-      <c r="AC48" s="3"/>
-      <c r="AD48" s="3"/>
-      <c r="AE48" s="3"/>
-      <c r="AF48" s="3"/>
-      <c r="AG48" s="3"/>
-      <c r="AH48" s="3"/>
-      <c r="AI48" s="3"/>
-      <c r="AJ48" s="3"/>
-      <c r="AK48" s="3"/>
-      <c r="AL48" s="3"/>
-      <c r="AM48" s="3"/>
-      <c r="AN48" s="3"/>
-      <c r="AO48" s="3"/>
-      <c r="AP48" s="3"/>
-      <c r="AQ48" s="3"/>
-      <c r="AR48" s="3"/>
-      <c r="AS48" s="3"/>
-      <c r="AT48" s="3"/>
-      <c r="AU48" s="3"/>
-      <c r="AV48" s="3"/>
-      <c r="AW48" s="3"/>
-      <c r="AX48" s="3"/>
-      <c r="AY48" s="3"/>
-      <c r="AZ48" s="3"/>
-      <c r="BA48" s="3"/>
-      <c r="BB48" s="3"/>
-      <c r="BC48" s="3"/>
-      <c r="BD48" s="3"/>
-      <c r="BE48" s="3"/>
-      <c r="BF48" s="3"/>
-      <c r="BG48" s="3"/>
-      <c r="BH48" s="3"/>
-      <c r="BI48" s="3"/>
-      <c r="BJ48" s="3"/>
-      <c r="BK48" s="3"/>
-      <c r="BL48" s="3"/>
-      <c r="BM48" s="3"/>
-      <c r="BN48" s="3"/>
-      <c r="BO48" s="3"/>
-      <c r="BP48" s="3"/>
-      <c r="BQ48" s="3"/>
-      <c r="BR48" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>